<commit_message>
final changes made to prac1
</commit_message>
<xml_diff>
--- a/3096-Pracs-ISLMDS002/Prac1/Lab1/Compileflags.xlsx
+++ b/3096-Pracs-ISLMDS002/Prac1/Lab1/Compileflags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UCT\Third_Year\Second Semester\EEE3096S\EEE3096S\3096-Pracs-ISLMDS002\Prac1\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76D94C1-BFF6-49B1-9262-598B3AC45F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20185F-7A8D-4FCF-930D-4BC638051BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="2430" windowWidth="13530" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Test Run</t>
   </si>
@@ -383,15 +383,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,20 +407,8 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -436,20 +424,8 @@
       <c r="E2">
         <v>3.2630699999999999</v>
       </c>
-      <c r="F2">
-        <v>2.8490700000000002</v>
-      </c>
-      <c r="G2">
-        <v>2.66107</v>
-      </c>
-      <c r="H2">
-        <v>18.173500000000001</v>
-      </c>
-      <c r="I2">
-        <v>3.1110899999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -465,20 +441,8 @@
       <c r="E3">
         <v>15.1012</v>
       </c>
-      <c r="F3">
-        <v>21.848299999999998</v>
-      </c>
-      <c r="G3">
-        <v>15.0732</v>
-      </c>
-      <c r="H3">
-        <v>3.1910400000000001</v>
-      </c>
-      <c r="I3">
-        <v>5.3539000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -494,20 +458,8 @@
       <c r="E4">
         <v>6.6380800000000004</v>
       </c>
-      <c r="F4">
-        <v>9.3791200000000003</v>
-      </c>
-      <c r="G4">
-        <v>4.87906</v>
-      </c>
-      <c r="H4">
-        <v>24.711300000000001</v>
-      </c>
-      <c r="I4">
-        <v>9.6128099999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -523,20 +475,8 @@
       <c r="E5">
         <v>26.224299999999999</v>
       </c>
-      <c r="F5">
-        <v>15.5472</v>
-      </c>
-      <c r="G5">
-        <v>2.4500299999999999</v>
-      </c>
-      <c r="H5">
-        <v>37.6845</v>
-      </c>
-      <c r="I5">
-        <v>6.94686</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -552,20 +492,8 @@
       <c r="E6">
         <v>19.5642</v>
       </c>
-      <c r="F6">
-        <v>10.4041</v>
-      </c>
-      <c r="G6">
-        <v>23.622299999999999</v>
-      </c>
-      <c r="H6">
-        <v>22.880299999999998</v>
-      </c>
-      <c r="I6">
-        <v>12.4917</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -585,20 +513,127 @@
         <f t="shared" si="0"/>
         <v>14.158170000000002</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>2.8490700000000002</v>
+      </c>
+      <c r="C10">
+        <v>2.66107</v>
+      </c>
+      <c r="D10">
+        <v>18.173500000000001</v>
+      </c>
+      <c r="E10">
+        <v>3.1110899999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>21.848299999999998</v>
+      </c>
+      <c r="C11">
+        <v>15.0732</v>
+      </c>
+      <c r="D11">
+        <v>3.1910400000000001</v>
+      </c>
+      <c r="E11">
+        <v>5.3539000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>9.3791200000000003</v>
+      </c>
+      <c r="C12">
+        <v>4.87906</v>
+      </c>
+      <c r="D12">
+        <v>24.711300000000001</v>
+      </c>
+      <c r="E12">
+        <v>9.6128099999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>15.5472</v>
+      </c>
+      <c r="C13">
+        <v>2.4500299999999999</v>
+      </c>
+      <c r="D13">
+        <v>37.6845</v>
+      </c>
+      <c r="E13">
+        <v>6.94686</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>10.4041</v>
+      </c>
+      <c r="C14">
+        <v>23.622299999999999</v>
+      </c>
+      <c r="D14">
+        <v>22.880299999999998</v>
+      </c>
+      <c r="E14">
+        <v>12.4917</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B10:B14)</f>
         <v>12.005557999999999</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
+      <c r="C15">
+        <f>AVERAGE(C10:C14)</f>
         <v>9.737131999999999</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
+      <c r="D15">
+        <f>AVERAGE(D10:D14)</f>
         <v>21.328128</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
+      <c r="E15">
+        <f>AVERAGE(E10:E14)</f>
         <v>7.5032719999999999</v>
       </c>
     </row>

</xml_diff>